<commit_message>
Remeasured BPA lengths and Max contraction
</commit_message>
<xml_diff>
--- a/DataCollection/BPAparameters.xlsx
+++ b/DataCollection/BPAparameters.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6F4125-4633-476B-B167-86B14A216D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFDCB09-3235-4D82-BB99-B854AFA34AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
-    <sheet name="20mm" sheetId="2" r:id="rId2"/>
+    <sheet name="10mm_Remeasured" sheetId="3" r:id="rId2"/>
+    <sheet name="20mm" sheetId="2" r:id="rId3"/>
+    <sheet name="20mm_Remeasured" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
   <si>
     <t>Resting Length(lo)</t>
   </si>
@@ -77,6 +79,9 @@
   <si>
     <t>20mm40cm</t>
   </si>
+  <si>
+    <t>Max Contraction( Resting Length - MaxPressure Length)</t>
+  </si>
 </sst>
 </file>
 
@@ -104,12 +109,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -204,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -230,6 +247,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,10 +570,728 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEF9700-E1C9-4441-A1F6-55B1B57CE96B}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E20"/>
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="31">
+        <v>13.5</v>
+      </c>
+      <c r="J2" s="2">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10</v>
+      </c>
+      <c r="L2" s="25">
+        <v>12</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6">
+        <v>11.6</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="26">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6">
+        <v>11.2</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="26">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9">
+        <v>10.8</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="27">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2">
+        <v>21.9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D6" s="11">
+        <v>21.9</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="32">
+        <v>23.6</v>
+      </c>
+      <c r="J6" s="2">
+        <v>21.9</v>
+      </c>
+      <c r="K6" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="L6" s="25">
+        <v>21.9</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="26">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="13">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="27">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>27.6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="D9" s="11">
+        <v>25.7</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="31">
+        <v>27.6</v>
+      </c>
+      <c r="J9" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="K9" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="L9" s="25">
+        <v>25.7</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="12">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="26">
+        <v>25</v>
+      </c>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="12">
+        <v>24.2</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="26">
+        <v>24.2</v>
+      </c>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="13">
+        <v>22.6</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="27">
+        <v>22.6</v>
+      </c>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>28.1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>23.6</v>
+      </c>
+      <c r="D13" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="31">
+        <v>29.8</v>
+      </c>
+      <c r="J13" s="2">
+        <v>28.1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>23.6</v>
+      </c>
+      <c r="L13" s="25">
+        <v>28.1</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="12">
+        <v>26.4</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="26">
+        <v>26.4</v>
+      </c>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="12">
+        <v>25.3</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="26">
+        <v>25.3</v>
+      </c>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="13">
+        <v>24</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="27">
+        <v>24</v>
+      </c>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>30</v>
+      </c>
+      <c r="B17" s="16">
+        <v>28.1</v>
+      </c>
+      <c r="C17" s="16">
+        <v>24</v>
+      </c>
+      <c r="D17" s="17">
+        <v>28.1</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="15">
+        <v>30</v>
+      </c>
+      <c r="J17" s="16">
+        <v>28.1</v>
+      </c>
+      <c r="K17" s="16">
+        <v>24</v>
+      </c>
+      <c r="L17" s="28">
+        <v>28.1</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="14">
+        <v>26.9</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="29">
+        <v>26.9</v>
+      </c>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="14">
+        <v>25.9</v>
+      </c>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="29">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22">
+        <v>24.8</v>
+      </c>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="30">
+        <v>24.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9872EE10-2925-48E3-A0F9-0084BA825885}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>13.7</v>
+      </c>
+      <c r="B2" s="33">
+        <v>12</v>
+      </c>
+      <c r="C2" s="33">
+        <v>10</v>
+      </c>
+      <c r="D2" s="25">
+        <v>12</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <f>B2-C2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="26">
+        <v>11.6</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G17" si="0">B3-C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="26">
+        <v>11.2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="27">
+        <v>10.8</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>23.7</v>
+      </c>
+      <c r="B6" s="33">
+        <v>22</v>
+      </c>
+      <c r="C6" s="33">
+        <v>18.5</v>
+      </c>
+      <c r="D6" s="25">
+        <v>21.9</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="26">
+        <v>20.5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="27">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>27.7</v>
+      </c>
+      <c r="B9" s="33">
+        <v>26</v>
+      </c>
+      <c r="C9" s="33">
+        <v>21.8</v>
+      </c>
+      <c r="D9" s="25">
+        <v>25.7</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>4.1999999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="26">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="26">
+        <v>24.2</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="27">
+        <v>22.6</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>29.7</v>
+      </c>
+      <c r="B13" s="33">
+        <v>28.1</v>
+      </c>
+      <c r="C13" s="33">
+        <v>23.5</v>
+      </c>
+      <c r="D13" s="25">
+        <v>28.1</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>4.6000000000000014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="26">
+        <v>26.4</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="26">
+        <v>25.3</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="27">
+        <v>24</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>30</v>
+      </c>
+      <c r="B17" s="16">
+        <v>28.1</v>
+      </c>
+      <c r="C17" s="16">
+        <v>24</v>
+      </c>
+      <c r="D17" s="28">
+        <v>28.1</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>4.1000000000000014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="29">
+        <v>26.9</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="29">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="30">
+        <v>24.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D771DB-D047-4EA9-B500-4A9CE86629AF}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +1302,7 @@
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -571,249 +1315,21 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="B2" s="2">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>12</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6">
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2">
-        <v>21.9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="D6" s="11">
-        <v>21.9</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="12">
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="13">
-        <v>18.899999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>27.6</v>
-      </c>
-      <c r="B9" s="2">
-        <v>25.7</v>
-      </c>
-      <c r="C9" s="2">
-        <v>22.1</v>
-      </c>
-      <c r="D9" s="11">
-        <v>25.7</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="12">
-        <v>25</v>
-      </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="12">
-        <v>24.2</v>
-      </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="13">
-        <v>22.6</v>
-      </c>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>29.8</v>
-      </c>
-      <c r="B13" s="2">
-        <v>28.1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>23.6</v>
-      </c>
-      <c r="D13" s="11">
-        <v>28.1</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="12">
-        <v>26.4</v>
-      </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="12">
-        <v>25.3</v>
-      </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="13">
-        <v>24</v>
-      </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <v>30</v>
-      </c>
-      <c r="B17" s="16">
-        <v>28.1</v>
-      </c>
-      <c r="C17" s="16">
-        <v>24</v>
-      </c>
-      <c r="D17" s="17">
-        <v>28.1</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="14">
-        <v>26.9</v>
-      </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="14">
-        <v>25.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22">
-        <v>24.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D771DB-D047-4EA9-B500-4A9CE86629AF}">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
         <v>12.4</v>
       </c>
       <c r="B2" s="2">
@@ -828,8 +1344,23 @@
       <c r="E2" s="23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="I2" s="2">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J2" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="K2" s="25">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -837,8 +1368,15 @@
         <v>8.5</v>
       </c>
       <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -846,9 +1384,16 @@
         <v>7.8</v>
       </c>
       <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="27">
+        <v>7.8</v>
+      </c>
+      <c r="L4" s="23"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
         <v>15</v>
       </c>
       <c r="B5" s="2">
@@ -863,8 +1408,23 @@
       <c r="E5" s="23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2">
+        <v>12</v>
+      </c>
+      <c r="J5" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="K5" s="25">
+        <v>12</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -872,8 +1432,15 @@
         <v>11</v>
       </c>
       <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="26">
+        <v>11</v>
+      </c>
+      <c r="L6" s="23"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -881,9 +1448,16 @@
         <v>10</v>
       </c>
       <c r="E7" s="23"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="27">
+        <v>10</v>
+      </c>
+      <c r="L7" s="23"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
         <v>25.3</v>
       </c>
       <c r="B8" s="2">
@@ -898,8 +1472,23 @@
       <c r="E8" s="23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <v>25.3</v>
+      </c>
+      <c r="I8" s="2">
+        <v>22.8</v>
+      </c>
+      <c r="J8" s="2">
+        <v>17.3</v>
+      </c>
+      <c r="K8" s="25">
+        <v>22.8</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -907,8 +1496,15 @@
         <v>21.9</v>
       </c>
       <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="26">
+        <v>21.9</v>
+      </c>
+      <c r="L9" s="23"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -916,9 +1512,16 @@
         <v>20.9</v>
       </c>
       <c r="E10" s="23"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="27">
+        <v>20.9</v>
+      </c>
+      <c r="L10" s="23"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
         <v>30</v>
       </c>
       <c r="B11" s="2">
@@ -933,8 +1536,23 @@
       <c r="E11" s="23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <v>30</v>
+      </c>
+      <c r="I11" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="J11" s="2">
+        <v>20.7</v>
+      </c>
+      <c r="K11" s="25">
+        <v>27.5</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -942,8 +1560,15 @@
         <v>26.1</v>
       </c>
       <c r="E12" s="23"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H12" s="4"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="26">
+        <v>26.1</v>
+      </c>
+      <c r="L12" s="23"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -951,8 +1576,15 @@
         <v>25.2</v>
       </c>
       <c r="E13" s="23"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="26">
+        <v>25.2</v>
+      </c>
+      <c r="L13" s="23"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -960,9 +1592,16 @@
         <v>24.1</v>
       </c>
       <c r="E14" s="23"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="27">
+        <v>24.1</v>
+      </c>
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
         <v>42.7</v>
       </c>
       <c r="B15" s="2">
@@ -977,8 +1616,23 @@
       <c r="E15" s="23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H15" s="1">
+        <v>42.7</v>
+      </c>
+      <c r="I15" s="2">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="J15" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="K15" s="25">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -986,8 +1640,15 @@
         <v>36.200000000000003</v>
       </c>
       <c r="E16" s="23"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="26">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="L16" s="23"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -995,8 +1656,15 @@
         <v>35.1</v>
       </c>
       <c r="E17" s="23"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="18"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="29">
+        <v>35.1</v>
+      </c>
+      <c r="L17" s="23"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -1004,15 +1672,22 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E18" s="23"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="30">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="24"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1022,4 +1697,285 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D860FA2-4E9F-49AC-BB20-38F305245ED7}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J21:J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>12.5</v>
+      </c>
+      <c r="B2" s="33">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C2" s="33">
+        <v>7.6</v>
+      </c>
+      <c r="D2" s="25">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <f>B2-C2</f>
+        <v>2.2000000000000011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="G3">
+        <f t="shared" ref="G3:G15" si="0">B3-C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="27">
+        <v>7.8</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>14.8</v>
+      </c>
+      <c r="B5" s="33">
+        <v>12</v>
+      </c>
+      <c r="C5" s="33">
+        <v>9.1</v>
+      </c>
+      <c r="D5" s="25">
+        <v>12</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.9000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="26">
+        <v>11</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="27">
+        <v>10</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <v>25.2</v>
+      </c>
+      <c r="B8" s="33">
+        <v>22.5</v>
+      </c>
+      <c r="C8" s="33">
+        <v>17</v>
+      </c>
+      <c r="D8" s="25">
+        <v>22.8</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="26">
+        <v>21.9</v>
+      </c>
+      <c r="E9" s="23"/>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="27">
+        <v>20.9</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>30</v>
+      </c>
+      <c r="B11" s="33">
+        <v>27.4</v>
+      </c>
+      <c r="C11" s="33">
+        <v>20.7</v>
+      </c>
+      <c r="D11" s="25">
+        <v>27.5</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>6.6999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="26">
+        <v>26.1</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="26">
+        <v>25.2</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="27">
+        <v>24.1</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
+        <v>42.6</v>
+      </c>
+      <c r="B15" s="33">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="C15" s="33">
+        <v>29.9</v>
+      </c>
+      <c r="D15" s="25">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>9.8999999999999986</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="26">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="29">
+        <v>35.1</v>
+      </c>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="30">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E18" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
separated plots for pressurizing and depressurizing
also included strains
</commit_message>
<xml_diff>
--- a/DataCollection/BPAparameters.xlsx
+++ b/DataCollection/BPAparameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AE9A7B-1194-4D9C-86C3-224F66FD96F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E46BEB-AEA4-4D84-A5B6-F5F174EC83DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
@@ -573,7 +573,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9872EE10-2925-48E3-A0F9-0084BA825885}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,11 +1705,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D860FA2-4E9F-49AC-BB20-38F305245ED7}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J21:J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
New max strain 10mm
</commit_message>
<xml_diff>
--- a/DataCollection/BPAparameters.xlsx
+++ b/DataCollection/BPAparameters.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory_2\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E46BEB-AEA4-4D84-A5B6-F5F174EC83DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A45BBF-7852-471E-BA6B-1CE4003400F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
     <sheet name="10mm_Remeasured" sheetId="3" r:id="rId2"/>
-    <sheet name="20mm" sheetId="2" r:id="rId3"/>
-    <sheet name="20mm_Remeasured" sheetId="4" r:id="rId4"/>
+    <sheet name="10mm_NewRecollectedData" sheetId="5" r:id="rId3"/>
+    <sheet name="20mm" sheetId="2" r:id="rId4"/>
+    <sheet name="20mm_Remeasured" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
   <si>
     <t>Resting Length(lo)</t>
   </si>
@@ -81,6 +82,27 @@
   </si>
   <si>
     <t>Max Contraction( Resting Length - MaxPressure Length)</t>
+  </si>
+  <si>
+    <t>pressire</t>
+  </si>
+  <si>
+    <t>641kPa</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>8.94kPa</t>
+  </si>
+  <si>
+    <t>Max Strain</t>
+  </si>
+  <si>
+    <t>Comment: these are measured without any constraints, measured free hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to recollect again on test jig for better reading(straighter BPA) </t>
   </si>
 </sst>
 </file>
@@ -221,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -256,6 +278,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,6 +299,935 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Resting length and max strain</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'10mm_NewRecollectedData'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'10mm_NewRecollectedData'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.15662650602409645</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15909090909090906</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16483516483516483</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17167381974248927</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17437722419928833</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17801047120418859</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.176056338028169</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-489E-41AD-9B40-F61768492F52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="380890112"/>
+        <c:axId val="380890440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="380890112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="380890440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="380890440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="380890112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B6E8CE8-15B1-68F0-215C-C6D10D55C78B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,7 +1530,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,6 +1583,10 @@
       <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
+      <c r="F2">
+        <f>A2-B2</f>
+        <v>1.5</v>
+      </c>
       <c r="I2" s="31">
         <v>13.5</v>
       </c>
@@ -649,6 +1610,10 @@
       <c r="D3" s="6">
         <v>11.6</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F20" si="0">A3-B3</f>
+        <v>0</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -663,6 +1628,14 @@
       <c r="D4" s="6">
         <v>11.2</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>+A210</f>
+        <v>0</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -677,6 +1650,10 @@
       <c r="D5" s="9">
         <v>10.8</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -699,6 +1676,10 @@
       </c>
       <c r="E6" s="10" t="s">
         <v>5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000014</v>
       </c>
       <c r="I6" s="32">
         <v>23.6</v>
@@ -723,6 +1704,10 @@
       <c r="D7" s="12">
         <v>20.5</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -737,6 +1722,10 @@
       <c r="D8" s="13">
         <v>18.899999999999999</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I8" s="7"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -759,6 +1748,10 @@
       </c>
       <c r="E9" s="10" t="s">
         <v>6</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1.9000000000000021</v>
       </c>
       <c r="I9" s="31">
         <v>27.6</v>
@@ -784,6 +1777,10 @@
         <v>25</v>
       </c>
       <c r="E10" s="10"/>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -800,6 +1797,10 @@
         <v>24.2</v>
       </c>
       <c r="E11" s="10"/>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -816,6 +1817,10 @@
         <v>22.6</v>
       </c>
       <c r="E12" s="10"/>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I12" s="7"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -839,6 +1844,10 @@
       </c>
       <c r="E13" s="10" t="s">
         <v>7</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1.6999999999999993</v>
       </c>
       <c r="I13" s="31">
         <v>29.8</v>
@@ -864,6 +1873,10 @@
         <v>26.4</v>
       </c>
       <c r="E14" s="10"/>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -880,6 +1893,10 @@
         <v>25.3</v>
       </c>
       <c r="E15" s="10"/>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -896,6 +1913,10 @@
         <v>24</v>
       </c>
       <c r="E16" s="10"/>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I16" s="7"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -919,6 +1940,10 @@
       </c>
       <c r="E17" s="10" t="s">
         <v>8</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1.8999999999999986</v>
       </c>
       <c r="I17" s="15">
         <v>30</v>
@@ -944,6 +1969,10 @@
         <v>26.9</v>
       </c>
       <c r="E18" s="10"/>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I18" s="18"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -959,6 +1988,10 @@
       <c r="D19" s="14">
         <v>25.9</v>
       </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I19" s="18"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -972,6 +2005,10 @@
       <c r="C20" s="21"/>
       <c r="D20" s="22">
         <v>24.8</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
@@ -991,7 +2028,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection sqref="A1:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,6 +2326,223 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6CD35F-74A9-469A-95AE-E3CD27253D58}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34">
+        <v>10</v>
+      </c>
+      <c r="B2" s="35">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C2" s="35">
+        <v>7</v>
+      </c>
+      <c r="D2" s="11">
+        <f>(B2-C2)/B2</f>
+        <v>0.15662650602409645</v>
+      </c>
+      <c r="E2">
+        <f>A2-B2</f>
+        <v>1.6999999999999993</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34">
+        <v>15</v>
+      </c>
+      <c r="B3" s="35">
+        <v>13.2</v>
+      </c>
+      <c r="C3" s="35">
+        <v>11.1</v>
+      </c>
+      <c r="D3" s="11">
+        <f>(B3-C3)/B3</f>
+        <v>0.15909090909090906</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" si="0">A3-B3</f>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="F3" s="37">
+        <v>639</v>
+      </c>
+      <c r="G3" s="37"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34">
+        <v>20</v>
+      </c>
+      <c r="B4" s="35">
+        <v>18.2</v>
+      </c>
+      <c r="C4" s="35">
+        <v>15.2</v>
+      </c>
+      <c r="D4" s="11">
+        <f>(B4-C4)/B4</f>
+        <v>0.16483516483516483</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="F4" s="37">
+        <v>640</v>
+      </c>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34">
+        <v>25</v>
+      </c>
+      <c r="B5" s="35">
+        <v>23.3</v>
+      </c>
+      <c r="C5" s="35">
+        <v>19.3</v>
+      </c>
+      <c r="D5" s="11">
+        <f>(B5-C5)/B5</f>
+        <v>0.17167381974248927</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.6999999999999993</v>
+      </c>
+      <c r="F5" s="37">
+        <v>640</v>
+      </c>
+      <c r="G5" s="37"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>30</v>
+      </c>
+      <c r="B6" s="39">
+        <v>28.1</v>
+      </c>
+      <c r="C6" s="39">
+        <v>23.2</v>
+      </c>
+      <c r="D6" s="17">
+        <f>(B6-C6)/B6</f>
+        <v>0.17437722419928833</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.8999999999999986</v>
+      </c>
+      <c r="F6" s="37">
+        <v>639</v>
+      </c>
+      <c r="G6" s="37"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="C7">
+        <v>31.4</v>
+      </c>
+      <c r="D7">
+        <f>(B7-C7)/B7</f>
+        <v>0.17801047120418859</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999972</v>
+      </c>
+      <c r="F7">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>44.5</v>
+      </c>
+      <c r="B8">
+        <v>42.6</v>
+      </c>
+      <c r="C8">
+        <v>35.1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8" si="1">(B8-C8)/B8</f>
+        <v>0.176056338028169</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.8999999999999986</v>
+      </c>
+      <c r="F8">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D771DB-D047-4EA9-B500-4A9CE86629AF}">
   <dimension ref="A1:L20"/>
   <sheetViews>
@@ -1701,12 +2955,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D860FA2-4E9F-49AC-BB20-38F305245ED7}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Collected all 10mm data (New)
</commit_message>
<xml_diff>
--- a/DataCollection/BPAparameters.xlsx
+++ b/DataCollection/BPAparameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory_2\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C37140-7497-422E-A143-FA9526EDADB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022C8EDD-BFD7-4D3E-93EA-392C7A515F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
   </bookViews>
@@ -234,7 +234,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,19 +355,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -401,11 +388,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -440,21 +442,105 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1452,15 +1538,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2586,1069 +2672,1165 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6CD35F-74A9-469A-95AE-E3CD27253D58}">
-  <dimension ref="B1:M47"/>
+  <dimension ref="B1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="6" width="47.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="34"/>
+    <col min="2" max="2" width="16.85546875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="34" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="34" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="34">
+      <c r="B2" s="35">
         <v>10</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="36">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="36">
         <v>7</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="36">
         <f t="shared" ref="E2:E7" si="0">(C2-D2)/C2</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F2" s="35">
+      <c r="F2" s="36">
         <f>C2-D2</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="37">
         <f>B2-C2</f>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="39" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="38">
+      <c r="B3" s="40">
         <v>15</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="41">
         <v>13.2</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="41">
         <v>11.1</v>
       </c>
-      <c r="E3" s="36">
+      <c r="E3" s="41">
         <f t="shared" si="0"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="41">
         <f t="shared" ref="F3:F8" si="1">C3-D3</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="42">
         <f t="shared" ref="G3:G8" si="2">B3-C3</f>
         <v>1.8000000000000007</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="41">
         <v>639</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="43" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="38">
+      <c r="B4" s="40">
         <v>20</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="41">
         <v>18.2</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="41">
         <v>15.2</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="41">
         <f t="shared" si="0"/>
         <v>0.16483516483516483</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="41">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="42">
         <f t="shared" si="2"/>
         <v>1.8000000000000007</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="41">
         <v>640</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="43" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="38">
+      <c r="B5" s="40">
         <v>25</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="41">
         <v>23.3</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="41">
         <v>19.3</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="41">
         <f t="shared" si="0"/>
         <v>0.17167381974248927</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="41">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="42">
         <f t="shared" si="2"/>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="41">
         <v>640</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="43" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="39">
+      <c r="B6" s="44">
         <v>30</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="45">
         <v>28.1</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="45">
         <v>23.2</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="45">
         <f t="shared" si="0"/>
         <v>0.17437722419928833</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="41">
         <f t="shared" si="1"/>
         <v>4.9000000000000021</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="42">
         <f t="shared" si="2"/>
         <v>1.8999999999999986</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="41">
         <v>639</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="43" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
+      <c r="B7" s="46">
         <v>40</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="42">
         <v>38.200000000000003</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="42">
         <v>31.4</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="42">
         <f t="shared" si="0"/>
         <v>0.17801047120418859</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="41">
         <f t="shared" si="1"/>
         <v>6.8000000000000043</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="42">
         <f t="shared" si="2"/>
         <v>1.7999999999999972</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="42">
         <v>640</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="43" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7">
+      <c r="B8" s="47">
         <v>44.5</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="48">
         <v>42.6</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="48">
         <v>35.1</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="48">
         <f t="shared" ref="E8" si="3">(C8-D8)/C8</f>
         <v>0.176056338028169</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="49">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="48">
         <f t="shared" si="2"/>
         <v>1.8999999999999986</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="48">
         <v>640</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="50" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="34" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="B16" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="34">
+      <c r="B17" s="35">
         <v>10</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="36">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="36">
         <v>7</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="36">
         <f t="shared" ref="E17:E23" si="4">(C17-D17)/C17</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="2">
+      <c r="F17" s="36"/>
+      <c r="G17" s="37">
         <f>B17-C17</f>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="38">
         <v>830</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="39" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="38">
+      <c r="B18" s="40">
         <v>15</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="41">
         <v>13.2</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="41">
         <v>11.1</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="41">
         <f t="shared" si="4"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="5">
+      <c r="F18" s="41"/>
+      <c r="G18" s="42">
         <f t="shared" ref="G18:G23" si="5">B18-C18</f>
         <v>1.8000000000000007</v>
       </c>
-      <c r="H18" s="36">
+      <c r="H18" s="41">
         <v>830</v>
       </c>
-      <c r="I18" s="12"/>
+      <c r="I18" s="43"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="38">
+      <c r="B19" s="40">
         <v>20</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36" t="e">
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="5">
+      <c r="F19" s="41"/>
+      <c r="G19" s="42">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="12"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="43"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="38">
+      <c r="B20" s="40">
         <v>25</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36" t="e">
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="5">
+      <c r="F20" s="41"/>
+      <c r="G20" s="42">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="H20" s="36"/>
-      <c r="I20" s="12"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="43"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="39">
+      <c r="B21" s="44">
         <v>30</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24" t="e">
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="5">
+      <c r="F21" s="45"/>
+      <c r="G21" s="42">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="H21" s="36"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
+      <c r="H21" s="41"/>
+      <c r="I21" s="43"/>
+    </row>
+    <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="46">
         <v>40</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="e">
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5">
+      <c r="F22" s="42"/>
+      <c r="G22" s="42">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="12"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
     </row>
     <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="7">
+      <c r="B23" s="51">
         <v>44.5</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="e">
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8">
+      <c r="F23" s="52"/>
+      <c r="G23" s="53">
         <f t="shared" si="5"/>
         <v>44.5</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="13"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="50"/>
     </row>
     <row r="25" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G25" t="s">
+      <c r="G25" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G26" s="41">
+      <c r="G26" s="54">
         <v>0.25</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G27" s="42">
+      <c r="G27" s="55">
         <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="B28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="42">
+      <c r="G28" s="55">
         <v>0.75</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="34" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="45" t="s">
+      <c r="D29" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="45" t="s">
+      <c r="E29" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="45" t="s">
+      <c r="F29" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="45" t="s">
+      <c r="G29" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="45" t="s">
+      <c r="H29" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="45" t="s">
+      <c r="I29" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="45" t="s">
+      <c r="J29" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="45" t="s">
+      <c r="K29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="L29" s="45" t="s">
+      <c r="L29" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="M29" s="46" t="s">
+      <c r="M29" s="58" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
+      <c r="B30" s="46">
         <v>10</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="41">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="41">
         <v>7</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="41">
         <f t="shared" ref="E30:E36" si="6">(C30-D30)/C30</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F30" s="36">
+      <c r="F30" s="41">
         <f>C30-D30</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="G30" s="4">
-        <f>$G$26*F30</f>
+      <c r="G30" s="59">
+        <f t="shared" ref="G30:G36" si="7">$G$26*F30</f>
         <v>0.32500000000000018</v>
       </c>
-      <c r="H30" s="42">
-        <f>$G$27*F30</f>
+      <c r="H30" s="54">
+        <f t="shared" ref="H30:H36" si="8">$G$27*F30</f>
         <v>0.65000000000000036</v>
       </c>
-      <c r="I30" s="6">
-        <f>$G$28*F30</f>
+      <c r="I30" s="60">
+        <f t="shared" ref="I30:I36" si="9">$G$28*F30</f>
         <v>0.97500000000000053</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="37">
         <f>C30</f>
         <v>8.3000000000000007</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="37">
         <f>C30-G30</f>
         <v>7.9750000000000005</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="37">
         <f>C30-H30</f>
         <v>7.65</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="60">
         <f>C30-I30</f>
         <v>7.3250000000000002</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="4">
+      <c r="B31" s="46">
         <v>15</v>
       </c>
-      <c r="C31" s="36">
+      <c r="C31" s="41">
         <v>13.2</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="41">
         <v>11.1</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="41">
         <f t="shared" si="6"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F31" s="36">
-        <f t="shared" ref="F31:F36" si="7">C31-D31</f>
+      <c r="F31" s="41">
+        <f t="shared" ref="F31:F36" si="10">C31-D31</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G31" s="4">
-        <f>$G$26*F31</f>
+      <c r="G31" s="46">
+        <f t="shared" si="7"/>
         <v>0.52499999999999991</v>
       </c>
-      <c r="H31" s="42">
-        <f>$G$27*F31</f>
+      <c r="H31" s="55">
+        <f t="shared" si="8"/>
         <v>1.0499999999999998</v>
       </c>
-      <c r="I31" s="6">
-        <f>$G$28*F31</f>
+      <c r="I31" s="61">
+        <f t="shared" si="9"/>
         <v>1.5749999999999997</v>
       </c>
-      <c r="J31">
-        <f t="shared" ref="J31:J36" si="8">C31</f>
+      <c r="J31" s="42">
+        <f t="shared" ref="J31:J36" si="11">C31</f>
         <v>13.2</v>
       </c>
-      <c r="K31">
-        <f t="shared" ref="K31:K36" si="9">C31-G31</f>
+      <c r="K31" s="42">
+        <f t="shared" ref="K31:K36" si="12">C31-G31</f>
         <v>12.674999999999999</v>
       </c>
-      <c r="L31">
-        <f t="shared" ref="L31:L36" si="10">C31-H31</f>
+      <c r="L31" s="42">
+        <f t="shared" ref="L31:L36" si="13">C31-H31</f>
         <v>12.149999999999999</v>
       </c>
-      <c r="M31">
-        <f t="shared" ref="M31:M36" si="11">C31-I31</f>
+      <c r="M31" s="61">
+        <f t="shared" ref="M31:M36" si="14">C31-I31</f>
         <v>11.625</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
+      <c r="B32" s="46">
         <v>20</v>
       </c>
-      <c r="C32" s="36">
+      <c r="C32" s="41">
         <v>18.2</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="41">
         <v>15.2</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="41">
         <f t="shared" si="6"/>
         <v>0.16483516483516483</v>
       </c>
-      <c r="F32" s="36">
+      <c r="F32" s="41">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="G32" s="46">
         <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="G32" s="4">
-        <f>$G$26*F32</f>
         <v>0.75</v>
       </c>
-      <c r="H32" s="42">
-        <f>$G$27*F32</f>
+      <c r="H32" s="55">
+        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
-      <c r="I32" s="6">
-        <f>$G$28*F32</f>
+      <c r="I32" s="61">
+        <f t="shared" si="9"/>
         <v>2.25</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="8"/>
+      <c r="J32" s="42">
+        <f t="shared" si="11"/>
         <v>18.2</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="9"/>
+      <c r="K32" s="42">
+        <f t="shared" si="12"/>
         <v>17.45</v>
       </c>
-      <c r="L32">
-        <f t="shared" si="10"/>
+      <c r="L32" s="42">
+        <f t="shared" si="13"/>
         <v>16.7</v>
       </c>
-      <c r="M32">
-        <f t="shared" si="11"/>
+      <c r="M32" s="61">
+        <f t="shared" si="14"/>
         <v>15.95</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="4">
+      <c r="B33" s="46">
         <v>25</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C33" s="41">
         <v>23.3</v>
       </c>
-      <c r="D33" s="36">
+      <c r="D33" s="41">
         <v>19.3</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="41">
         <f t="shared" si="6"/>
         <v>0.17167381974248927</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="41">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="G33" s="46">
         <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="G33" s="4">
-        <f>$G$26*F33</f>
         <v>1</v>
       </c>
-      <c r="H33" s="42">
-        <f>$G$27*F33</f>
+      <c r="H33" s="55">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="I33" s="6">
-        <f>$G$28*F33</f>
+      <c r="I33" s="61">
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="J33">
-        <f t="shared" si="8"/>
+      <c r="J33" s="42">
+        <f t="shared" si="11"/>
         <v>23.3</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="9"/>
+      <c r="K33" s="42">
+        <f t="shared" si="12"/>
         <v>22.3</v>
       </c>
-      <c r="L33">
-        <f t="shared" si="10"/>
+      <c r="L33" s="42">
+        <f t="shared" si="13"/>
         <v>21.3</v>
       </c>
-      <c r="M33">
-        <f t="shared" si="11"/>
+      <c r="M33" s="61">
+        <f t="shared" si="14"/>
         <v>20.3</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
+      <c r="B34" s="46">
         <v>30</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="45">
         <v>28.1</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="45">
         <v>23.2</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="45">
         <f t="shared" si="6"/>
         <v>0.17437722419928833</v>
       </c>
-      <c r="F34" s="36">
+      <c r="F34" s="41">
+        <f t="shared" si="10"/>
+        <v>4.9000000000000021</v>
+      </c>
+      <c r="G34" s="46">
         <f t="shared" si="7"/>
-        <v>4.9000000000000021</v>
-      </c>
-      <c r="G34" s="4">
-        <f>$G$26*F34</f>
         <v>1.2250000000000005</v>
       </c>
-      <c r="H34" s="42">
-        <f>$G$27*F34</f>
+      <c r="H34" s="55">
+        <f t="shared" si="8"/>
         <v>2.4500000000000011</v>
       </c>
-      <c r="I34" s="6">
-        <f>$G$28*F34</f>
+      <c r="I34" s="61">
+        <f t="shared" si="9"/>
         <v>3.6750000000000016</v>
       </c>
-      <c r="J34">
-        <f t="shared" si="8"/>
+      <c r="J34" s="42">
+        <f t="shared" si="11"/>
         <v>28.1</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="9"/>
+      <c r="K34" s="42">
+        <f t="shared" si="12"/>
         <v>26.875</v>
       </c>
-      <c r="L34">
-        <f t="shared" si="10"/>
+      <c r="L34" s="42">
+        <f t="shared" si="13"/>
         <v>25.65</v>
       </c>
-      <c r="M34">
-        <f t="shared" si="11"/>
+      <c r="M34" s="61">
+        <f t="shared" si="14"/>
         <v>24.425000000000001</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
+    <row r="35" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="46">
         <v>40</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="42">
         <v>38.200000000000003</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="42">
         <v>31.4</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="42">
         <f t="shared" si="6"/>
         <v>0.17801047120418859</v>
       </c>
-      <c r="F35" s="36">
+      <c r="F35" s="41">
+        <f t="shared" si="10"/>
+        <v>6.8000000000000043</v>
+      </c>
+      <c r="G35" s="46">
         <f t="shared" si="7"/>
-        <v>6.8000000000000043</v>
-      </c>
-      <c r="G35" s="4">
-        <f>$G$26*F35</f>
         <v>1.7000000000000011</v>
       </c>
-      <c r="H35" s="42">
-        <f>$G$27*F35</f>
+      <c r="H35" s="55">
+        <f t="shared" si="8"/>
         <v>3.4000000000000021</v>
       </c>
-      <c r="I35" s="6">
-        <f>$G$28*F35</f>
+      <c r="I35" s="61">
+        <f t="shared" si="9"/>
         <v>5.1000000000000032</v>
       </c>
-      <c r="J35">
-        <f t="shared" si="8"/>
+      <c r="J35" s="42">
+        <f t="shared" si="11"/>
         <v>38.200000000000003</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="9"/>
+      <c r="K35" s="42">
+        <f t="shared" si="12"/>
         <v>36.5</v>
       </c>
-      <c r="L35">
-        <f t="shared" si="10"/>
+      <c r="L35" s="42">
+        <f t="shared" si="13"/>
         <v>34.799999999999997</v>
       </c>
-      <c r="M35">
-        <f t="shared" si="11"/>
+      <c r="M35" s="61">
+        <f t="shared" si="14"/>
         <v>33.1</v>
       </c>
     </row>
     <row r="36" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="7">
+      <c r="B36" s="51">
         <v>44.5</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="52">
         <v>42.6</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="52">
         <v>35.1</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="52">
         <f t="shared" si="6"/>
         <v>0.176056338028169</v>
       </c>
-      <c r="F36" s="40">
+      <c r="F36" s="52">
+        <f t="shared" si="10"/>
+        <v>7.5</v>
+      </c>
+      <c r="G36" s="51">
         <f t="shared" si="7"/>
-        <v>7.5</v>
-      </c>
-      <c r="G36" s="7">
-        <f>$G$26*F36</f>
         <v>1.875</v>
       </c>
-      <c r="H36" s="43">
-        <f>$G$27*F36</f>
+      <c r="H36" s="62">
+        <f t="shared" si="8"/>
         <v>3.75</v>
       </c>
-      <c r="I36" s="9">
-        <f>$G$28*F36</f>
+      <c r="I36" s="53">
+        <f t="shared" si="9"/>
         <v>5.625</v>
       </c>
-      <c r="J36">
-        <f t="shared" si="8"/>
+      <c r="J36" s="52">
+        <f t="shared" si="11"/>
         <v>42.6</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="9"/>
+      <c r="K36" s="52">
+        <f t="shared" si="12"/>
         <v>40.725000000000001</v>
       </c>
-      <c r="L36">
-        <f t="shared" si="10"/>
+      <c r="L36" s="52">
+        <f t="shared" si="13"/>
         <v>38.85</v>
       </c>
-      <c r="M36">
-        <f t="shared" si="11"/>
+      <c r="M36" s="53">
+        <f t="shared" si="14"/>
         <v>36.975000000000001</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G38" t="s">
+      <c r="G38" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38" s="34" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+      <c r="B39" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="34">
         <v>40.6</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E40" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="45" t="s">
+      <c r="F40" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="45" t="s">
+      <c r="G40" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="H40" s="45" t="s">
+      <c r="H40" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="I40" s="45" t="s">
+      <c r="I40" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="J40" s="46" t="s">
+      <c r="J40" s="58" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="4">
+      <c r="B41" s="46">
         <v>10</v>
       </c>
-      <c r="C41" s="36">
+      <c r="C41" s="41">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="41">
         <v>7</v>
       </c>
-      <c r="E41" s="36">
-        <f t="shared" ref="E41:E47" si="12">(C41-D41)/C41</f>
+      <c r="E41" s="41">
+        <f t="shared" ref="E41:E48" si="15">(C41-D41)/C41</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F41" s="36">
+      <c r="F41" s="41">
         <f>C41-D41</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="46">
         <f>$G$39</f>
         <v>40.6</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="42">
         <f>$G$39-G30</f>
         <v>40.274999999999999</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="42">
         <f>$G$39-H30</f>
         <v>39.950000000000003</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="61">
         <f>$G$39-I30</f>
         <v>39.625</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="4">
+      <c r="B42" s="46">
         <v>15</v>
       </c>
-      <c r="C42" s="36">
+      <c r="C42" s="41">
         <v>13.2</v>
       </c>
-      <c r="D42" s="36">
+      <c r="D42" s="41">
         <v>11.1</v>
       </c>
-      <c r="E42" s="36">
-        <f t="shared" si="12"/>
+      <c r="E42" s="41">
+        <f t="shared" si="15"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F42" s="36">
-        <f t="shared" ref="F42:F47" si="13">C42-D42</f>
+      <c r="F42" s="41">
+        <f t="shared" ref="F42:F48" si="16">C42-D42</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G42" s="36">
+      <c r="G42" s="40">
         <v>45.3</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="42">
         <f>$G$42-G31</f>
         <v>44.774999999999999</v>
       </c>
-      <c r="I42" s="5">
-        <f t="shared" ref="I42:J42" si="14">$G$42-H31</f>
+      <c r="I42" s="42">
+        <f t="shared" ref="I42:J42" si="17">$G$42-H31</f>
         <v>44.25</v>
       </c>
-      <c r="J42" s="5">
-        <f t="shared" si="14"/>
+      <c r="J42" s="61">
+        <f t="shared" si="17"/>
         <v>43.724999999999994</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="4">
+      <c r="B43" s="46">
         <v>20</v>
       </c>
-      <c r="C43" s="36">
+      <c r="C43" s="41">
         <v>18.2</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="41">
         <v>15.2</v>
       </c>
-      <c r="E43" s="36">
-        <f t="shared" si="12"/>
+      <c r="E43" s="41">
+        <f t="shared" si="15"/>
         <v>0.16483516483516483</v>
       </c>
-      <c r="F43" s="36">
-        <f t="shared" si="13"/>
+      <c r="F43" s="41">
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
+      <c r="G43" s="40">
+        <v>50.5</v>
+      </c>
+      <c r="H43" s="42">
+        <f>G43-G32</f>
+        <v>49.75</v>
+      </c>
+      <c r="I43" s="42">
+        <f>G43-H32</f>
+        <v>49</v>
+      </c>
+      <c r="J43" s="61">
+        <f>G43-I32</f>
+        <v>48.25</v>
+      </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="4">
+      <c r="B44" s="46">
         <v>25</v>
       </c>
-      <c r="C44" s="36">
+      <c r="C44" s="41">
         <v>23.3</v>
       </c>
-      <c r="D44" s="36">
+      <c r="D44" s="41">
         <v>19.3</v>
       </c>
-      <c r="E44" s="36">
-        <f t="shared" si="12"/>
+      <c r="E44" s="41">
+        <f t="shared" si="15"/>
         <v>0.17167381974248927</v>
       </c>
-      <c r="F44" s="36">
-        <f t="shared" si="13"/>
+      <c r="F44" s="41">
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
+      <c r="G44" s="40">
+        <v>55.6</v>
+      </c>
+      <c r="H44" s="42">
+        <f>$G$44-G33</f>
+        <v>54.6</v>
+      </c>
+      <c r="I44" s="42">
+        <f t="shared" ref="I44:J44" si="18">$G$44-H33</f>
+        <v>53.6</v>
+      </c>
+      <c r="J44" s="61">
+        <f t="shared" si="18"/>
+        <v>52.6</v>
+      </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="4">
+      <c r="B45" s="46">
         <v>30</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="45">
         <v>28.1</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="45">
         <v>23.2</v>
       </c>
-      <c r="E45" s="24">
-        <f t="shared" si="12"/>
+      <c r="E45" s="45">
+        <f t="shared" si="15"/>
         <v>0.17437722419928833</v>
       </c>
-      <c r="F45" s="36">
-        <f t="shared" si="13"/>
+      <c r="F45" s="41">
+        <f t="shared" si="16"/>
         <v>4.9000000000000021</v>
       </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
+      <c r="G45" s="44">
+        <v>60.5</v>
+      </c>
+      <c r="H45" s="42">
+        <f>$G$45-G34</f>
+        <v>59.274999999999999</v>
+      </c>
+      <c r="I45" s="42">
+        <f>$G$45-H34</f>
+        <v>58.05</v>
+      </c>
+      <c r="J45" s="61">
+        <f>$G$45-I34</f>
+        <v>56.824999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="47">
         <v>40</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="48">
         <v>38.200000000000003</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="48">
         <v>31.4</v>
       </c>
-      <c r="E46" s="5">
-        <f t="shared" si="12"/>
+      <c r="E46" s="48">
+        <f t="shared" si="15"/>
         <v>0.17801047120418859</v>
       </c>
-      <c r="F46" s="36">
-        <f t="shared" si="13"/>
+      <c r="F46" s="49">
+        <f t="shared" si="16"/>
         <v>6.8000000000000043</v>
       </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
+      <c r="G46" s="63">
+        <v>70.7</v>
+      </c>
+      <c r="H46" s="48">
+        <f>$G$46-G35</f>
+        <v>69</v>
+      </c>
+      <c r="I46" s="48">
+        <f t="shared" ref="I46:J46" si="19">$G$46-H35</f>
+        <v>67.3</v>
+      </c>
+      <c r="J46" s="64">
+        <f t="shared" si="19"/>
+        <v>65.599999999999994</v>
+      </c>
     </row>
     <row r="47" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="47">
+      <c r="B47" s="51">
         <v>44.5</v>
       </c>
-      <c r="C47" s="48">
+      <c r="C47" s="52">
         <v>42.6</v>
       </c>
-      <c r="D47" s="48">
+      <c r="D47" s="52">
         <v>35.1</v>
       </c>
-      <c r="E47" s="48">
-        <f t="shared" si="12"/>
+      <c r="E47" s="52">
+        <f t="shared" si="15"/>
         <v>0.176056338028169</v>
       </c>
-      <c r="F47" s="48">
-        <f t="shared" si="13"/>
+      <c r="F47" s="52">
+        <f t="shared" si="16"/>
         <v>7.5</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
+      <c r="G47" s="51">
+        <v>10000</v>
+      </c>
+      <c r="H47" s="52">
+        <f>$G$47-G26*F47</f>
+        <v>9998.125</v>
+      </c>
+      <c r="I47" s="52">
+        <f>$G$47-G27*F47</f>
+        <v>9996.25</v>
+      </c>
+      <c r="J47" s="52">
+        <f>$G$47-G28*F47</f>
+        <v>9994.375</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="65"/>
+      <c r="C48" s="66">
+        <v>52.1</v>
+      </c>
+      <c r="D48" s="66">
+        <v>43.7</v>
+      </c>
+      <c r="E48" s="66">
+        <f t="shared" si="15"/>
+        <v>0.16122840690978885</v>
+      </c>
+      <c r="F48" s="66">
+        <f t="shared" si="16"/>
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="G48" s="65">
+        <v>84.5</v>
+      </c>
+      <c r="H48" s="66">
+        <f>$G$48-G26*F48</f>
+        <v>82.4</v>
+      </c>
+      <c r="I48" s="66">
+        <f>$G$48-G27*F48</f>
+        <v>80.3</v>
+      </c>
+      <c r="J48" s="66">
+        <f>$G$48-G28*F48</f>
+        <v>78.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>